<commit_message>
docs(report): correct BUG_PROD_001 from invalid XSS to UI/UX missing keyword issue and update severity metrics
</commit_message>
<xml_diff>
--- a/Bug Reports/Master_Bug_List.xlsx
+++ b/Bug Reports/Master_Bug_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Downloads\hockyVII\kiem_thu_phan_mem\bai_tap\MANUAL-TESTING-GROUP-3\Bug Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7694CFED-6AAD-4A05-BE76-55DE23B772D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2822038D-1B58-49CE-B9A5-56028E9AB55F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{EBFA1372-7861-4427-83A2-144EE943A471}"/>
   </bookViews>
@@ -152,18 +152,6 @@
     <t>Phải có nút "Quên mật khẩu" để người dùng đặt lại mật khẩu khi cần.</t>
   </si>
   <si>
-    <t>TC_PROD_004</t>
-  </si>
-  <si>
-    <t>Lỗ hổng XSS (Chèn mã HTML) trên thanh Tìm kiếm sản phẩm</t>
-  </si>
-  <si>
-    <t>Đoạn mã HTML bị thực thi, chữ "Lỗi" in đậm khổng lồ xuất hiện trên màn hình.</t>
-  </si>
-  <si>
-    <t>Trình duyệt phải mã hóa (Encode) ký tự đặc biệt, không thực thi mã HTML.</t>
-  </si>
-  <si>
     <t>TC_PROD_012</t>
   </si>
   <si>
@@ -251,11 +239,6 @@
 2. Quan sát biểu mẫu Đăng nhập (Login form)</t>
   </si>
   <si>
-    <t>1. Vào trang Products
-2. Nhập &lt;h1&gt;Lỗi&lt;/h1&gt; vào ô Search
-3. Nhấn Tìm kiếm</t>
-  </si>
-  <si>
     <t>1. Vào trang Chi tiết sản phẩm
 2. Tại mục Review, nhập Email qamail.com
 3. Nhấn Submit</t>
@@ -282,6 +265,23 @@
   <si>
     <t>1. Đặt hàng thành công
 2. Tìm trang theo dõi đơn hàng trên thanh Menu và Profile</t>
+  </si>
+  <si>
+    <t>TC_PROD_001</t>
+  </si>
+  <si>
+    <t>[Cập nhật] Lỗi UX: Không hiển thị lại từ khóa đã tìm kiếm trên màn hình kết quả</t>
+  </si>
+  <si>
+    <t>1. Vào trang Products
+2. Nhập từ khóa bất kỳ vào ô Search
+3. Nhấn Tìm kiếm</t>
+  </si>
+  <si>
+    <t>Tiêu đề chỉ hiển thị chung chung là "SEARCHED PRODUCTS", không chứa từ khóa người dùng đã nhập.</t>
+  </si>
+  <si>
+    <t>Phải hiển thị rõ từ khóa để người dùng xác nhận, VD: "SEARCHED PRODUCTS FOR 'Blue Top'".</t>
   </si>
 </sst>
 </file>
@@ -429,7 +429,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -459,76 +469,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF434343"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFF6F8F9"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FFFFFFFF"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF356854"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -731,6 +671,56 @@
       </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF434343"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFF6F8F9"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FFFFFFFF"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF356854"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -745,18 +735,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{68A1717B-08D1-4DDB-85BD-8F5D5C1B805C}" name="Table2" displayName="Table2" ref="A1:I11" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{68A1717B-08D1-4DDB-85BD-8F5D5C1B805C}" name="Table2" displayName="Table2" ref="A1:I11" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A1:I11" xr:uid="{68A1717B-08D1-4DDB-85BD-8F5D5C1B805C}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{40428921-833A-4B26-8F0D-DC5DD9DC6BA2}" name="Mã lỗi (Bug ID)" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{B182CF14-B4C5-4860-BEB0-5E618DA3B5BE}" name="Mã kịch bản (TC_ID)" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{CE0964A4-EEED-4511-9BFA-DDDFDC34CC5B}" name="Tiêu đề lỗi (Bug Summary)" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{64228DFA-D164-4AB4-8F4D-08B0BB7A81E6}" name="Mức độ (Severity)" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{BF6D1AEB-119C-40FE-9B61-6C587CB8AAE1}" name="Ưu tiên (Priority)" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{7713A2F3-7B3B-4CFF-B1B1-B624A332B858}" name="Các bước tái hiện (Steps to Reproduce)" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{36A7FC87-93A9-49DB-9EBE-A197FCB689A5}" name="Kết quả thực tế (Actual Result)" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{B0707D9E-2E4E-4C1E-8DEE-957DE97FA592}" name="Kết quả mong đợi (Expected Result)" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{BB994078-BA38-48D7-97B5-6D0029FF98D9}" name="Trạng thái (Status)" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{40428921-833A-4B26-8F0D-DC5DD9DC6BA2}" name="Mã lỗi (Bug ID)" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{B182CF14-B4C5-4860-BEB0-5E618DA3B5BE}" name="Mã kịch bản (TC_ID)" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{CE0964A4-EEED-4511-9BFA-DDDFDC34CC5B}" name="Tiêu đề lỗi (Bug Summary)" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{64228DFA-D164-4AB4-8F4D-08B0BB7A81E6}" name="Mức độ (Severity)" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{BF6D1AEB-119C-40FE-9B61-6C587CB8AAE1}" name="Ưu tiên (Priority)" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{7713A2F3-7B3B-4CFF-B1B1-B624A332B858}" name="Các bước tái hiện (Steps to Reproduce)" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{36A7FC87-93A9-49DB-9EBE-A197FCB689A5}" name="Kết quả thực tế (Actual Result)" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{B0707D9E-2E4E-4C1E-8DEE-957DE97FA592}" name="Kết quả mong đợi (Expected Result)" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{BB994078-BA38-48D7-97B5-6D0029FF98D9}" name="Trạng thái (Status)" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1081,8 +1071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC46C5B2-93F3-428C-8160-6EA21A8AE1F5}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1144,7 +1134,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>28</v>
@@ -1173,7 +1163,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>32</v>
@@ -1202,7 +1192,7 @@
         <v>7</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>36</v>
@@ -1214,30 +1204,30 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="46.15" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>8</v>
@@ -1248,10 +1238,10 @@
         <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>10</v>
@@ -1260,13 +1250,13 @@
         <v>11</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>8</v>
@@ -1280,7 +1270,7 @@
         <v>18</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>6</v>
@@ -1289,13 +1279,13 @@
         <v>7</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>8</v>
@@ -1306,10 +1296,10 @@
         <v>19</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>13</v>
@@ -1318,13 +1308,13 @@
         <v>7</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>8</v>
@@ -1332,13 +1322,13 @@
     </row>
     <row r="9" spans="1:9" ht="61.5" x14ac:dyDescent="0.45">
       <c r="A9" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>10</v>
@@ -1347,13 +1337,13 @@
         <v>16</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>8</v>
@@ -1364,10 +1354,10 @@
         <v>20</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>13</v>
@@ -1376,13 +1366,13 @@
         <v>7</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>8</v>
@@ -1393,10 +1383,10 @@
         <v>21</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>6</v>
@@ -1405,38 +1395,33 @@
         <v>7</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Major">
+  <conditionalFormatting sqref="D2:D11">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="cri">
+      <formula>NOT(ISERROR(SEARCH("cri",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Minor">
+      <formula>NOT(ISERROR(SEARCH("Minor",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="Major">
       <formula>NOT(ISERROR(SEARCH("Major",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",D3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D11">
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Major">
-      <formula>NOT(ISERROR(SEARCH("Major",D2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Minor">
-      <formula>NOT(ISERROR(SEARCH("Minor",D2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="cri">
-      <formula>NOT(ISERROR(SEARCH("cri",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>